<commit_message>
In the maps, use quintiles from CSV files, not our own calculations: New CSV file for IN23 Highest qualification
</commit_message>
<xml_diff>
--- a/son/content/intermediate_outcomes/routes_into_work_(16_to_29_years)/highest_qualification/2.0/IN23-2.0-highest-qualification--by-ITL2-region--chart-format.xlsx
+++ b/son/content/intermediate_outcomes/routes_into_work_(16_to_29_years)/highest_qualification/2.0/IN23-2.0-highest-qualification--by-ITL2-region--chart-format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\intermediate_outcomes\routes_into_work_(16_to_29_years)\highest_qualification\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{64178D2D-0C82-4A9F-BD6A-D4A45B24CCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB4B466-0B00-43CD-8A82-2C85E63BF172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{34464CDB-25C4-4A16-A55D-7BA3934774F8}"/>
+    <workbookView xWindow="11715" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{34464CDB-25C4-4A16-A55D-7BA3934774F8}"/>
   </bookViews>
   <sheets>
     <sheet name="IN23-2.0-highest-qualification-" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3632" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="104">
   <si>
     <t>ind_code</t>
   </si>
@@ -7259,7 +7259,7 @@
         <v>30</v>
       </c>
       <c r="N98">
-        <v>17.889999528152501</v>
+        <v>17.889999528152401</v>
       </c>
       <c r="O98">
         <v>341</v>
@@ -7271,7 +7271,7 @@
         <v>0.190681041264645</v>
       </c>
       <c r="R98">
-        <v>3.9910719185168898E-2</v>
+        <v>3.9910719185169301E-2</v>
       </c>
       <c r="S98" t="s">
         <v>31</v>
@@ -7321,19 +7321,19 @@
         <v>30</v>
       </c>
       <c r="N99">
-        <v>62.406172169635397</v>
+        <v>62.406172169635099</v>
       </c>
       <c r="O99">
         <v>1094</v>
       </c>
       <c r="P99">
-        <v>0.60729633562499796</v>
+        <v>0.60729633562499497</v>
       </c>
       <c r="Q99">
-        <v>0.64053501705363802</v>
+        <v>0.64053501705363503</v>
       </c>
       <c r="R99">
-        <v>3.6153560969595898E-2</v>
+        <v>3.6153560969595801E-2</v>
       </c>
       <c r="S99" t="s">
         <v>31</v>
@@ -7383,19 +7383,19 @@
         <v>30</v>
       </c>
       <c r="N100">
-        <v>32.105772550715201</v>
+        <v>32.105772550715102</v>
       </c>
       <c r="O100">
         <v>9</v>
       </c>
       <c r="P100">
-        <v>0.25069941301464099</v>
+        <v>0.25069941301463999</v>
       </c>
       <c r="Q100">
-        <v>0.40060502957767502</v>
+        <v>0.40060502957767402</v>
       </c>
       <c r="R100">
-        <v>0.176511158066225</v>
+        <v>0.176511158066226</v>
       </c>
       <c r="S100" t="s">
         <v>31</v>
@@ -7445,16 +7445,16 @@
         <v>30</v>
       </c>
       <c r="N101">
-        <v>78.274361939113305</v>
+        <v>78.274361939113106</v>
       </c>
       <c r="O101">
         <v>4</v>
       </c>
       <c r="P101">
-        <v>0.71786994284518402</v>
+        <v>0.71786994284518102</v>
       </c>
       <c r="Q101">
-        <v>0.83610577716105705</v>
+        <v>0.83610577716105605</v>
       </c>
       <c r="R101">
         <v>0.17744809163460101</v>
@@ -7507,19 +7507,19 @@
         <v>30</v>
       </c>
       <c r="N102">
-        <v>31.960591487195</v>
+        <v>31.9605914871949</v>
       </c>
       <c r="O102">
         <v>16</v>
       </c>
       <c r="P102">
-        <v>0.26728954245428199</v>
+        <v>0.26728954245428099</v>
       </c>
       <c r="Q102">
-        <v>0.37689491338246001</v>
+        <v>0.37689491338245901</v>
       </c>
       <c r="R102">
-        <v>0.128994104259745</v>
+        <v>0.128994104259746</v>
       </c>
       <c r="S102" t="s">
         <v>31</v>
@@ -7569,16 +7569,16 @@
         <v>30</v>
       </c>
       <c r="N103">
-        <v>78.160750104433106</v>
+        <v>78.160750104432907</v>
       </c>
       <c r="O103">
         <v>17</v>
       </c>
       <c r="P103">
-        <v>0.73548225113370203</v>
+        <v>0.73548225113370003</v>
       </c>
       <c r="Q103">
-        <v>0.82164017308163595</v>
+        <v>0.82164017308163495</v>
       </c>
       <c r="R103">
         <v>0.12879312787465899</v>
@@ -7631,19 +7631,19 @@
         <v>30</v>
       </c>
       <c r="N104">
-        <v>19.047016272792298</v>
+        <v>19.047016272792199</v>
       </c>
       <c r="O104">
         <v>4</v>
       </c>
       <c r="P104">
-        <v>0.14777585897939899</v>
+        <v>0.14777585897939799</v>
       </c>
       <c r="Q104">
-        <v>0.24199677490285501</v>
+        <v>0.24199677490285401</v>
       </c>
       <c r="R104">
-        <v>0.15570781721761701</v>
+        <v>0.15570781721761601</v>
       </c>
       <c r="S104" t="s">
         <v>31</v>
@@ -7693,19 +7693,19 @@
         <v>30</v>
       </c>
       <c r="N105">
-        <v>64.191469276722103</v>
+        <v>64.191469276721705</v>
       </c>
       <c r="O105">
         <v>8</v>
       </c>
       <c r="P105">
-        <v>0.56934268618856398</v>
+        <v>0.56934268618856099</v>
       </c>
       <c r="Q105">
-        <v>0.70851826787268302</v>
+        <v>0.70851826787268002</v>
       </c>
       <c r="R105">
-        <v>0.15536063301434999</v>
+        <v>0.15536063301434899</v>
       </c>
       <c r="S105" t="s">
         <v>31</v>
@@ -7755,19 +7755,19 @@
         <v>30</v>
       </c>
       <c r="N106">
-        <v>58.242535326829604</v>
+        <v>58.242535326829099</v>
       </c>
       <c r="O106">
         <v>1</v>
       </c>
       <c r="P106">
-        <v>0.48519144231153399</v>
+        <v>0.485191442311531</v>
       </c>
       <c r="Q106">
-        <v>0.67364707763599097</v>
+        <v>0.67364707763598497</v>
       </c>
       <c r="R106">
-        <v>0.199989600137705</v>
+        <v>0.19998960013770101</v>
       </c>
       <c r="S106" t="s">
         <v>31</v>
@@ -7817,19 +7817,19 @@
         <v>30</v>
       </c>
       <c r="N107">
-        <v>91.399187801710994</v>
+        <v>91.399187801710795</v>
       </c>
       <c r="O107">
         <v>20</v>
       </c>
       <c r="P107">
-        <v>0.87802811996423402</v>
+        <v>0.87802811996423202</v>
       </c>
       <c r="Q107">
-        <v>0.94007533410316102</v>
+        <v>0.94007533410315902</v>
       </c>
       <c r="R107">
-        <v>0.19871544430994401</v>
+        <v>0.19871544430994001</v>
       </c>
       <c r="S107" t="s">
         <v>31</v>
@@ -7879,19 +7879,19 @@
         <v>30</v>
       </c>
       <c r="N108">
-        <v>49.231517643617998</v>
+        <v>49.231517643618403</v>
       </c>
       <c r="O108">
         <v>21</v>
       </c>
       <c r="P108">
-        <v>0.44203303466960497</v>
+        <v>0.44203303466960803</v>
       </c>
       <c r="Q108">
-        <v>0.54275327307574806</v>
+        <v>0.54275327307575305</v>
       </c>
       <c r="R108">
-        <v>0.103147167796538</v>
+        <v>0.10314716779654</v>
       </c>
       <c r="S108" t="s">
         <v>31</v>
@@ -7941,19 +7941,19 @@
         <v>30</v>
       </c>
       <c r="N109">
-        <v>88.078663399996103</v>
+        <v>88.078663399996202</v>
       </c>
       <c r="O109">
         <v>63</v>
       </c>
       <c r="P109">
-        <v>0.85792414274538897</v>
+        <v>0.85792414274538997</v>
       </c>
       <c r="Q109">
-        <v>0.90039726967729405</v>
+        <v>0.90039726967729505</v>
       </c>
       <c r="R109">
-        <v>0.102929082895798</v>
+        <v>0.10292908289579999</v>
       </c>
       <c r="S109" t="s">
         <v>31</v>
@@ -8003,19 +8003,19 @@
         <v>30</v>
       </c>
       <c r="N110">
-        <v>29.832380593019899</v>
+        <v>29.8323805930197</v>
       </c>
       <c r="O110">
         <v>16</v>
       </c>
       <c r="P110">
-        <v>0.25707715197172498</v>
+        <v>0.25707715197172298</v>
       </c>
       <c r="Q110">
-        <v>0.34313171762948402</v>
+        <v>0.34313171762948202</v>
       </c>
       <c r="R110">
-        <v>0.10506038171514499</v>
+        <v>0.10506038171514399</v>
       </c>
       <c r="S110" t="s">
         <v>31</v>
@@ -8065,16 +8065,16 @@
         <v>30</v>
       </c>
       <c r="N111">
-        <v>76.411063828307604</v>
+        <v>76.411063828307306</v>
       </c>
       <c r="O111">
         <v>32</v>
       </c>
       <c r="P111">
-        <v>0.725095154818722</v>
+        <v>0.725095154818718</v>
       </c>
       <c r="Q111">
-        <v>0.79912290991993695</v>
+        <v>0.79912290991993395</v>
       </c>
       <c r="R111">
         <v>0.10482998611146201</v>
@@ -8127,19 +8127,19 @@
         <v>30</v>
       </c>
       <c r="N112">
-        <v>29.2429852263584</v>
+        <v>29.242985226358201</v>
       </c>
       <c r="O112">
         <v>7</v>
       </c>
       <c r="P112">
-        <v>0.25643312428852699</v>
+        <v>0.25643312428852599</v>
       </c>
       <c r="Q112">
-        <v>0.33122869196487498</v>
+        <v>0.33122869196487198</v>
       </c>
       <c r="R112">
-        <v>9.2333872934967101E-2</v>
+        <v>9.2333872934966907E-2</v>
       </c>
       <c r="S112" t="s">
         <v>31</v>
@@ -8189,19 +8189,19 @@
         <v>30</v>
       </c>
       <c r="N113">
-        <v>75.896806924833598</v>
+        <v>75.896806924833299</v>
       </c>
       <c r="O113">
         <v>60</v>
       </c>
       <c r="P113">
-        <v>0.72506847979700095</v>
+        <v>0.72506847979699796</v>
       </c>
       <c r="Q113">
-        <v>0.78989896702677997</v>
+        <v>0.78989896702677798</v>
       </c>
       <c r="R113">
-        <v>9.0449933500105995E-2</v>
+        <v>9.0449933500105495E-2</v>
       </c>
       <c r="S113" t="s">
         <v>31</v>
@@ -8251,19 +8251,19 @@
         <v>30</v>
       </c>
       <c r="N114">
-        <v>25.895372421320399</v>
+        <v>25.895372421320101</v>
       </c>
       <c r="O114">
         <v>29</v>
       </c>
       <c r="P114">
-        <v>0.219165314851899</v>
+        <v>0.219165314851896</v>
       </c>
       <c r="Q114">
-        <v>0.30316102699469899</v>
+        <v>0.30316102699469499</v>
       </c>
       <c r="R114">
-        <v>0.111794926849864</v>
+        <v>0.111794926849862</v>
       </c>
       <c r="S114" t="s">
         <v>31</v>
@@ -8313,19 +8313,19 @@
         <v>30</v>
       </c>
       <c r="N115">
-        <v>72.695511643718206</v>
+        <v>72.695511643717794</v>
       </c>
       <c r="O115">
         <v>22</v>
       </c>
       <c r="P115">
-        <v>0.68135685864404205</v>
+        <v>0.68135685864403805</v>
       </c>
       <c r="Q115">
-        <v>0.768247632923309</v>
+        <v>0.768247632923304</v>
       </c>
       <c r="R115">
-        <v>0.11184120329531599</v>
+        <v>0.111841203295314</v>
       </c>
       <c r="S115" t="s">
         <v>31</v>
@@ -8375,19 +8375,19 @@
         <v>30</v>
       </c>
       <c r="N116">
-        <v>24.125748540751399</v>
+        <v>24.1257485407512</v>
       </c>
       <c r="O116">
         <v>45</v>
       </c>
       <c r="P116">
-        <v>0.21999985072806499</v>
+        <v>0.219999850728063</v>
       </c>
       <c r="Q116">
-        <v>0.263874273373082</v>
+        <v>0.26387427337308</v>
       </c>
       <c r="R116">
-        <v>6.11564199686567E-2</v>
+        <v>6.1156419968656499E-2</v>
       </c>
       <c r="S116" t="s">
         <v>31</v>
@@ -8437,19 +8437,19 @@
         <v>30</v>
       </c>
       <c r="N117">
-        <v>70.782512131017796</v>
+        <v>70.782512131017398</v>
       </c>
       <c r="O117">
         <v>100</v>
       </c>
       <c r="P117">
-        <v>0.68282767103920805</v>
+        <v>0.68282767103920405</v>
       </c>
       <c r="Q117">
-        <v>0.731626762595179</v>
+        <v>0.73162676259517601</v>
       </c>
       <c r="R117">
-        <v>6.0226717245502298E-2</v>
+        <v>6.0226717245501799E-2</v>
       </c>
       <c r="S117" t="s">
         <v>31</v>
@@ -12209,8 +12209,8 @@
       <c r="J178" t="s">
         <v>60</v>
       </c>
-      <c r="K178" t="s">
-        <v>30</v>
+      <c r="K178">
+        <v>5</v>
       </c>
       <c r="L178" t="s">
         <v>30</v>
@@ -12219,19 +12219,19 @@
         <v>30</v>
       </c>
       <c r="N178">
-        <v>3.26175598949576</v>
+        <v>3.2617551319973801</v>
       </c>
       <c r="O178">
         <v>346</v>
       </c>
       <c r="P178">
-        <v>-0.86124323319475105</v>
+        <v>-0.86124353304661605</v>
       </c>
       <c r="Q178">
-        <v>7.3847552121862599</v>
+        <v>7.3847537970413804</v>
       </c>
       <c r="R178">
-        <v>2.10357103198495E-2</v>
+        <v>2.10357074747143E-2</v>
       </c>
       <c r="S178" t="s">
         <v>61</v>
@@ -12271,8 +12271,8 @@
       <c r="J179" t="s">
         <v>60</v>
       </c>
-      <c r="K179" t="s">
-        <v>30</v>
+      <c r="K179">
+        <v>4</v>
       </c>
       <c r="L179" t="s">
         <v>30</v>
@@ -12281,19 +12281,19 @@
         <v>30</v>
       </c>
       <c r="N179">
-        <v>0.300806354384136</v>
+        <v>0.30080631895701498</v>
       </c>
       <c r="O179">
         <v>477</v>
       </c>
       <c r="P179">
-        <v>-3.3914562461506002</v>
+        <v>-3.3914558815955802</v>
       </c>
       <c r="Q179">
-        <v>3.99306895491888</v>
+        <v>3.9930685195096101</v>
       </c>
       <c r="R179">
-        <v>1.8838074492524198E-2</v>
+        <v>1.8838072451798901E-2</v>
       </c>
       <c r="S179" t="s">
         <v>61</v>
@@ -12333,8 +12333,8 @@
       <c r="J180" t="s">
         <v>60</v>
       </c>
-      <c r="K180" t="s">
-        <v>30</v>
+      <c r="K180">
+        <v>5</v>
       </c>
       <c r="L180" t="s">
         <v>30</v>
@@ -12343,19 +12343,19 @@
         <v>30</v>
       </c>
       <c r="N180">
-        <v>3.8852505496397498</v>
+        <v>3.88524903801199</v>
       </c>
       <c r="O180">
         <v>176</v>
       </c>
       <c r="P180">
-        <v>-1.08402023813686</v>
+        <v>-1.0840207718560699</v>
       </c>
       <c r="Q180">
-        <v>8.8545213374163705</v>
+        <v>8.8545188478800494</v>
       </c>
       <c r="R180">
-        <v>2.53534223866154E-2</v>
+        <v>2.5353417397285999E-2</v>
       </c>
       <c r="S180" t="s">
         <v>61</v>
@@ -12395,8 +12395,8 @@
       <c r="J181" t="s">
         <v>60</v>
       </c>
-      <c r="K181" t="s">
-        <v>30</v>
+      <c r="K181">
+        <v>2</v>
       </c>
       <c r="L181" t="s">
         <v>30</v>
@@ -12405,19 +12405,19 @@
         <v>30</v>
       </c>
       <c r="N181">
-        <v>-1.6100280790539701</v>
+        <v>-1.6100272561282301</v>
       </c>
       <c r="O181">
         <v>99</v>
       </c>
       <c r="P181">
-        <v>-7.2032452993317602</v>
+        <v>-7.20324308090174</v>
       </c>
       <c r="Q181">
-        <v>3.9831891412238298</v>
+        <v>3.9831885686452799</v>
       </c>
       <c r="R181">
-        <v>2.85368225524377E-2</v>
+        <v>2.85368154325179E-2</v>
       </c>
       <c r="S181" t="s">
         <v>61</v>
@@ -12457,8 +12457,8 @@
       <c r="J182" t="s">
         <v>60</v>
       </c>
-      <c r="K182" t="s">
-        <v>30</v>
+      <c r="K182">
+        <v>2</v>
       </c>
       <c r="L182" t="s">
         <v>30</v>
@@ -12467,19 +12467,19 @@
         <v>30</v>
       </c>
       <c r="N182">
-        <v>-1.5312282679087901</v>
+        <v>-1.5312275655426799</v>
       </c>
       <c r="O182">
         <v>133</v>
       </c>
       <c r="P182">
-        <v>-6.8016823127530497</v>
+        <v>-6.8016804432115601</v>
       </c>
       <c r="Q182">
-        <v>3.73922577693547</v>
+        <v>3.73922531212621</v>
       </c>
       <c r="R182">
-        <v>2.6890071657368699E-2</v>
+        <v>2.6890065702392298E-2</v>
       </c>
       <c r="S182" t="s">
         <v>61</v>
@@ -12519,8 +12519,8 @@
       <c r="J183" t="s">
         <v>60</v>
       </c>
-      <c r="K183" t="s">
-        <v>30</v>
+      <c r="K183">
+        <v>1</v>
       </c>
       <c r="L183" t="s">
         <v>30</v>
@@ -12529,19 +12529,19 @@
         <v>30</v>
       </c>
       <c r="N183">
-        <v>-3.5138657860938598</v>
+        <v>-3.5138649266207</v>
       </c>
       <c r="O183">
         <v>430</v>
       </c>
       <c r="P183">
-        <v>-7.3408214157962197</v>
+        <v>-7.3408201107514603</v>
       </c>
       <c r="Q183">
-        <v>0.313089843608513</v>
+        <v>0.31309025751004599</v>
       </c>
       <c r="R183">
-        <v>1.9525283825012101E-2</v>
+        <v>1.95252815516875E-2</v>
       </c>
       <c r="S183" t="s">
         <v>61</v>
@@ -12581,8 +12581,8 @@
       <c r="J184" t="s">
         <v>60</v>
       </c>
-      <c r="K184" t="s">
-        <v>30</v>
+      <c r="K184">
+        <v>4</v>
       </c>
       <c r="L184" t="s">
         <v>30</v>
@@ -12591,19 +12591,19 @@
         <v>30</v>
       </c>
       <c r="N184">
-        <v>1.26458383833601</v>
+        <v>1.26458344355095</v>
       </c>
       <c r="O184">
         <v>248</v>
       </c>
       <c r="P184">
-        <v>-3.3057503023271999</v>
+        <v>-3.3057499368173602</v>
       </c>
       <c r="Q184">
-        <v>5.8349179789992096</v>
+        <v>5.8349168239192499</v>
       </c>
       <c r="R184">
-        <v>2.33180313299143E-2</v>
+        <v>2.3318027450858699E-2</v>
       </c>
       <c r="S184" t="s">
         <v>61</v>
@@ -12643,8 +12643,8 @@
       <c r="J185" t="s">
         <v>60</v>
       </c>
-      <c r="K185" t="s">
-        <v>30</v>
+      <c r="K185">
+        <v>2</v>
       </c>
       <c r="L185" t="s">
         <v>30</v>
@@ -12653,19 +12653,19 @@
         <v>30</v>
       </c>
       <c r="N185">
-        <v>-1.60250079864384</v>
+        <v>-1.6025002713551599</v>
       </c>
       <c r="O185">
         <v>275</v>
       </c>
       <c r="P185">
-        <v>-6.0112399085990704</v>
+        <v>-6.0112386990584996</v>
       </c>
       <c r="Q185">
-        <v>2.80623831131139</v>
+        <v>2.80623815634819</v>
       </c>
       <c r="R185">
-        <v>2.2493566887526701E-2</v>
+        <v>2.2493563406649701E-2</v>
       </c>
       <c r="S185" t="s">
         <v>61</v>
@@ -12705,8 +12705,8 @@
       <c r="J186" t="s">
         <v>60</v>
       </c>
-      <c r="K186" t="s">
-        <v>30</v>
+      <c r="K186">
+        <v>1</v>
       </c>
       <c r="L186" t="s">
         <v>30</v>
@@ -12715,19 +12715,19 @@
         <v>30</v>
       </c>
       <c r="N186">
-        <v>-3.7402976780789001</v>
+        <v>-3.7402968286224798</v>
       </c>
       <c r="O186">
         <v>485</v>
       </c>
       <c r="P186">
-        <v>-7.4238864734569399</v>
+        <v>-7.4238852268427804</v>
       </c>
       <c r="Q186">
-        <v>-5.6708882700856597E-2</v>
+        <v>-5.6708430402181702E-2</v>
       </c>
       <c r="R186">
-        <v>1.87938203845819E-2</v>
+        <v>1.8793818358266799E-2</v>
       </c>
       <c r="S186" t="s">
         <v>61</v>
@@ -12767,8 +12767,8 @@
       <c r="J187" t="s">
         <v>60</v>
       </c>
-      <c r="K187" t="s">
-        <v>30</v>
+      <c r="K187">
+        <v>3</v>
       </c>
       <c r="L187" t="s">
         <v>30</v>
@@ -12777,19 +12777,19 @@
         <v>30</v>
       </c>
       <c r="N187">
-        <v>-0.32173597947654498</v>
+        <v>-0.32173584160306601</v>
       </c>
       <c r="O187">
         <v>224</v>
       </c>
       <c r="P187">
-        <v>-4.9538310971356401</v>
+        <v>-4.95383016763786</v>
       </c>
       <c r="Q187">
-        <v>4.3103591381825499</v>
+        <v>4.3103584844317302</v>
       </c>
       <c r="R187">
-        <v>2.36331383554035E-2</v>
+        <v>2.3633134316504101E-2</v>
       </c>
       <c r="S187" t="s">
         <v>61</v>
@@ -12829,8 +12829,8 @@
       <c r="J188" t="s">
         <v>60</v>
       </c>
-      <c r="K188" t="s">
-        <v>30</v>
+      <c r="K188">
+        <v>2</v>
       </c>
       <c r="L188" t="s">
         <v>30</v>
@@ -12839,19 +12839,19 @@
         <v>30</v>
       </c>
       <c r="N188">
-        <v>-1.7267970498193499</v>
+        <v>-1.7267963630224901</v>
       </c>
       <c r="O188">
         <v>189</v>
       </c>
       <c r="P188">
-        <v>-6.6133030318263097</v>
+        <v>-6.6133014152869301</v>
       </c>
       <c r="Q188">
-        <v>3.1597089321876002</v>
+        <v>3.1597086892419401</v>
       </c>
       <c r="R188">
-        <v>2.49311529694232E-2</v>
+        <v>2.4931148225839E-2</v>
       </c>
       <c r="S188" t="s">
         <v>61</v>
@@ -12891,8 +12891,8 @@
       <c r="J189" t="s">
         <v>60</v>
       </c>
-      <c r="K189" t="s">
-        <v>30</v>
+      <c r="K189">
+        <v>4</v>
       </c>
       <c r="L189" t="s">
         <v>30</v>
@@ -12901,19 +12901,19 @@
         <v>30</v>
       </c>
       <c r="N189">
-        <v>0.24630751768716599</v>
+        <v>0.24630748261354601</v>
       </c>
       <c r="O189">
         <v>352</v>
       </c>
       <c r="P189">
-        <v>-3.8329573853225698</v>
+        <v>-3.8329568803680201</v>
       </c>
       <c r="Q189">
-        <v>4.3255724206968997</v>
+        <v>4.3255718455951104</v>
       </c>
       <c r="R189">
-        <v>2.0812576035763902E-2</v>
+        <v>2.08125732805182E-2</v>
       </c>
       <c r="S189" t="s">
         <v>61</v>
@@ -12953,8 +12953,8 @@
       <c r="J190" t="s">
         <v>60</v>
       </c>
-      <c r="K190" t="s">
-        <v>30</v>
+      <c r="K190">
+        <v>4</v>
       </c>
       <c r="L190" t="s">
         <v>30</v>
@@ -12963,19 +12963,19 @@
         <v>30</v>
       </c>
       <c r="N190">
-        <v>1.0612787082540001</v>
+        <v>1.06127844901059</v>
       </c>
       <c r="O190">
         <v>333</v>
       </c>
       <c r="P190">
-        <v>-3.06982437265812</v>
+        <v>-3.0698240709489499</v>
       </c>
       <c r="Q190">
-        <v>5.1923817891661201</v>
+        <v>5.1923809689701201</v>
       </c>
       <c r="R190">
-        <v>2.1077056535265901E-2</v>
+        <v>2.1077053673262899E-2</v>
       </c>
       <c r="S190" t="s">
         <v>61</v>
@@ -13015,8 +13015,8 @@
       <c r="J191" t="s">
         <v>60</v>
       </c>
-      <c r="K191" t="s">
-        <v>30</v>
+      <c r="K191">
+        <v>3</v>
       </c>
       <c r="L191" t="s">
         <v>30</v>
@@ -13025,19 +13025,19 @@
         <v>30</v>
       </c>
       <c r="N191">
-        <v>-0.42044190971947099</v>
+        <v>-0.42044179018018502</v>
       </c>
       <c r="O191">
         <v>542</v>
       </c>
       <c r="P191">
-        <v>-3.9249570344128499</v>
+        <v>-3.9249565731009501</v>
       </c>
       <c r="Q191">
-        <v>3.0840732149739098</v>
+        <v>3.0840729927405799</v>
       </c>
       <c r="R191">
-        <v>1.78801792076193E-2</v>
+        <v>1.7880177463881399E-2</v>
       </c>
       <c r="S191" t="s">
         <v>61</v>
@@ -13077,8 +13077,8 @@
       <c r="J192" t="s">
         <v>60</v>
       </c>
-      <c r="K192" t="s">
-        <v>30</v>
+      <c r="K192">
+        <v>2</v>
       </c>
       <c r="L192" t="s">
         <v>30</v>
@@ -13087,19 +13087,19 @@
         <v>30</v>
       </c>
       <c r="N192">
-        <v>-1.6159651935894901</v>
+        <v>-1.61596479596708</v>
       </c>
       <c r="O192">
         <v>483</v>
       </c>
       <c r="P192">
-        <v>-5.3555459207278302</v>
+        <v>-5.3555451074798199</v>
       </c>
       <c r="Q192">
-        <v>2.1236155335488598</v>
+        <v>2.12361551554566</v>
       </c>
       <c r="R192">
-        <v>1.9079493505807898E-2</v>
+        <v>1.9079491385269098E-2</v>
       </c>
       <c r="S192" t="s">
         <v>61</v>
@@ -13139,8 +13139,8 @@
       <c r="J193" t="s">
         <v>60</v>
       </c>
-      <c r="K193" t="s">
-        <v>30</v>
+      <c r="K193">
+        <v>1</v>
       </c>
       <c r="L193" t="s">
         <v>30</v>
@@ -13149,19 +13149,19 @@
         <v>30</v>
       </c>
       <c r="N193">
-        <v>-3.7937231562728799</v>
+        <v>-3.79372212912364</v>
       </c>
       <c r="O193">
         <v>356</v>
       </c>
       <c r="P193">
-        <v>-7.8535636327730698</v>
+        <v>-7.8535620733004601</v>
       </c>
       <c r="Q193">
-        <v>0.266117320227303</v>
+        <v>0.266117815053177</v>
       </c>
       <c r="R193">
-        <v>2.07134718188785E-2</v>
+        <v>2.0713469102943E-2</v>
       </c>
       <c r="S193" t="s">
         <v>61</v>
@@ -13201,8 +13201,8 @@
       <c r="J194" t="s">
         <v>60</v>
       </c>
-      <c r="K194" t="s">
-        <v>30</v>
+      <c r="K194">
+        <v>4</v>
       </c>
       <c r="L194" t="s">
         <v>30</v>
@@ -13211,19 +13211,19 @@
         <v>30</v>
       </c>
       <c r="N194">
-        <v>1.2392696439047199</v>
+        <v>1.2392692745960301</v>
       </c>
       <c r="O194">
         <v>264</v>
       </c>
       <c r="P194">
-        <v>-3.2454842452396102</v>
+        <v>-3.2454838962852501</v>
       </c>
       <c r="Q194">
-        <v>5.7240235330490501</v>
+        <v>5.7240224454773001</v>
       </c>
       <c r="R194">
-        <v>2.2881397393593499E-2</v>
+        <v>2.2881393728986101E-2</v>
       </c>
       <c r="S194" t="s">
         <v>61</v>
@@ -13263,8 +13263,8 @@
       <c r="J195" t="s">
         <v>60</v>
       </c>
-      <c r="K195" t="s">
-        <v>30</v>
+      <c r="K195">
+        <v>3</v>
       </c>
       <c r="L195" t="s">
         <v>30</v>
@@ -13273,19 +13273,19 @@
         <v>30</v>
       </c>
       <c r="N195">
-        <v>-0.16438648220582</v>
+        <v>-0.16438637849511001</v>
       </c>
       <c r="O195">
         <v>69</v>
       </c>
       <c r="P195">
-        <v>-6.0633822573269702</v>
+        <v>-6.0633805160321996</v>
       </c>
       <c r="Q195">
-        <v>5.7346092929153301</v>
+        <v>5.7346077590419799</v>
       </c>
       <c r="R195">
-        <v>3.00969172200059E-2</v>
+        <v>3.00969088649852E-2</v>
       </c>
       <c r="S195" t="s">
         <v>61</v>
@@ -13325,8 +13325,8 @@
       <c r="J196" t="s">
         <v>60</v>
       </c>
-      <c r="K196" t="s">
-        <v>30</v>
+      <c r="K196">
+        <v>5</v>
       </c>
       <c r="L196" t="s">
         <v>30</v>
@@ -13335,19 +13335,19 @@
         <v>30</v>
       </c>
       <c r="N196">
-        <v>7.8898458070249502</v>
+        <v>7.8898429445286196</v>
       </c>
       <c r="O196">
         <v>211</v>
       </c>
       <c r="P196">
-        <v>3.1075221372642301</v>
+        <v>3.1075201461603399</v>
       </c>
       <c r="Q196">
-        <v>12.672169476785699</v>
+        <v>12.672165742896899</v>
       </c>
       <c r="R196">
-        <v>2.4399610560003698E-2</v>
+        <v>2.4399606114123899E-2</v>
       </c>
       <c r="S196" t="s">
         <v>61</v>
@@ -13387,8 +13387,8 @@
       <c r="J197" t="s">
         <v>60</v>
       </c>
-      <c r="K197" t="s">
-        <v>30</v>
+      <c r="K197">
+        <v>5</v>
       </c>
       <c r="L197" t="s">
         <v>30</v>
@@ -13397,19 +13397,19 @@
         <v>30</v>
       </c>
       <c r="N197">
-        <v>4.0493192841327597</v>
+        <v>4.0493172882548603</v>
       </c>
       <c r="O197">
         <v>102</v>
       </c>
       <c r="P197">
-        <v>-1.52383398668544</v>
+        <v>-1.52383460205106</v>
       </c>
       <c r="Q197">
-        <v>9.62247255495096</v>
+        <v>9.6224691785607792</v>
       </c>
       <c r="R197">
-        <v>2.84344554633582E-2</v>
+        <v>2.8434448419928201E-2</v>
       </c>
       <c r="S197" t="s">
         <v>61</v>
@@ -13449,8 +13449,8 @@
       <c r="J198" t="s">
         <v>60</v>
       </c>
-      <c r="K198" t="s">
-        <v>30</v>
+      <c r="K198">
+        <v>3</v>
       </c>
       <c r="L198" t="s">
         <v>30</v>
@@ -13459,19 +13459,19 @@
         <v>30</v>
       </c>
       <c r="N198">
-        <v>-0.31365855447409002</v>
+        <v>-0.31365843630086299</v>
       </c>
       <c r="O198">
         <v>322</v>
       </c>
       <c r="P198">
-        <v>-4.51991361692843</v>
+        <v>-4.5199129065198997</v>
       </c>
       <c r="Q198">
-        <v>3.89259650798025</v>
+        <v>3.89259603391818</v>
       </c>
       <c r="R198">
-        <v>2.1460485012522099E-2</v>
+        <v>2.1460481990913501E-2</v>
       </c>
       <c r="S198" t="s">
         <v>61</v>
@@ -13511,8 +13511,8 @@
       <c r="J199" t="s">
         <v>60</v>
       </c>
-      <c r="K199" t="s">
-        <v>30</v>
+      <c r="K199">
+        <v>3</v>
       </c>
       <c r="L199" t="s">
         <v>30</v>
@@ -13521,19 +13521,19 @@
         <v>30</v>
       </c>
       <c r="N199">
-        <v>-0.188991475082224</v>
+        <v>-0.188991387128712</v>
       </c>
       <c r="O199">
         <v>328</v>
       </c>
       <c r="P199">
-        <v>-4.3781919063549104</v>
+        <v>-4.3781912333645199</v>
       </c>
       <c r="Q199">
-        <v>4.0002089561904599</v>
+        <v>4.0002084591070899</v>
       </c>
       <c r="R199">
-        <v>2.13734715881259E-2</v>
+        <v>2.1373468603243899E-2</v>
       </c>
       <c r="S199" t="s">
         <v>61</v>
@@ -13573,8 +13573,8 @@
       <c r="J200" t="s">
         <v>60</v>
       </c>
-      <c r="K200" t="s">
-        <v>30</v>
+      <c r="K200">
+        <v>4</v>
       </c>
       <c r="L200" t="s">
         <v>30</v>
@@ -13583,19 +13583,19 @@
         <v>30</v>
       </c>
       <c r="N200">
-        <v>0.43080135350244803</v>
+        <v>0.43080126979491401</v>
       </c>
       <c r="O200">
         <v>364</v>
       </c>
       <c r="P200">
-        <v>-3.6367755428629698</v>
+        <v>-3.6367750911872698</v>
       </c>
       <c r="Q200">
-        <v>4.4983782498678604</v>
+        <v>4.4983776307771004</v>
       </c>
       <c r="R200">
-        <v>2.07529433488031E-2</v>
+        <v>2.0752940617256001E-2</v>
       </c>
       <c r="S200" t="s">
         <v>61</v>
@@ -13635,8 +13635,8 @@
       <c r="J201" t="s">
         <v>60</v>
       </c>
-      <c r="K201" t="s">
-        <v>30</v>
+      <c r="K201">
+        <v>1</v>
       </c>
       <c r="L201" t="s">
         <v>30</v>
@@ -13645,19 +13645,19 @@
         <v>30</v>
       </c>
       <c r="N201">
-        <v>-3.1419186057564601</v>
+        <v>-3.14191729872373</v>
       </c>
       <c r="O201">
         <v>161</v>
       </c>
       <c r="P201">
-        <v>-8.1908719199900393</v>
+        <v>-8.1908695871335002</v>
       </c>
       <c r="Q201">
-        <v>1.90703470847712</v>
+        <v>1.9070349896860499</v>
       </c>
       <c r="R201">
-        <v>2.5759965888946801E-2</v>
+        <v>2.57599606551519E-2</v>
       </c>
       <c r="S201" t="s">
         <v>61</v>
@@ -13697,8 +13697,8 @@
       <c r="J202" t="s">
         <v>60</v>
       </c>
-      <c r="K202" t="s">
-        <v>30</v>
+      <c r="K202">
+        <v>4</v>
       </c>
       <c r="L202" t="s">
         <v>30</v>
@@ -13707,19 +13707,19 @@
         <v>30</v>
       </c>
       <c r="N202">
-        <v>2.0893797565510099</v>
+        <v>2.0893791345291901</v>
       </c>
       <c r="O202">
         <v>273</v>
       </c>
       <c r="P202">
-        <v>-2.3292717591326002</v>
+        <v>-2.32927169427641</v>
       </c>
       <c r="Q202">
-        <v>6.5080312722346303</v>
+        <v>6.5080299633347902</v>
       </c>
       <c r="R202">
-        <v>2.2544140386140901E-2</v>
+        <v>2.2544136881661202E-2</v>
       </c>
       <c r="S202" t="s">
         <v>61</v>
@@ -13759,8 +13759,8 @@
       <c r="J203" t="s">
         <v>60</v>
       </c>
-      <c r="K203" t="s">
-        <v>30</v>
+      <c r="K203">
+        <v>1</v>
       </c>
       <c r="L203" t="s">
         <v>30</v>
@@ -13769,19 +13769,19 @@
         <v>30</v>
       </c>
       <c r="N203">
-        <v>-1.83087692455479</v>
+        <v>-1.83087597218093</v>
       </c>
       <c r="O203">
         <v>89</v>
       </c>
       <c r="P203">
-        <v>-7.48561165644497</v>
+        <v>-7.4856092619250898</v>
       </c>
       <c r="Q203">
-        <v>3.8238578073353899</v>
+        <v>3.82385731756324</v>
       </c>
       <c r="R203">
-        <v>2.8850687407603E-2</v>
+        <v>2.88506800497151E-2</v>
       </c>
       <c r="S203" t="s">
         <v>61</v>
@@ -13821,8 +13821,8 @@
       <c r="J204" t="s">
         <v>60</v>
       </c>
-      <c r="K204" t="s">
-        <v>30</v>
+      <c r="K204">
+        <v>5</v>
       </c>
       <c r="L204" t="s">
         <v>30</v>
@@ -13831,19 +13831,19 @@
         <v>30</v>
       </c>
       <c r="N204">
-        <v>4.0621147148061496</v>
+        <v>4.0621131825438201</v>
       </c>
       <c r="O204">
         <v>185</v>
       </c>
       <c r="P204">
-        <v>-0.83113089934905604</v>
+        <v>-0.83113149800709196</v>
       </c>
       <c r="Q204">
-        <v>8.9553603289613495</v>
+        <v>8.9553578630947293</v>
       </c>
       <c r="R204">
-        <v>2.49655388477306E-2</v>
+        <v>2.4965534084443401E-2</v>
       </c>
       <c r="S204" t="s">
         <v>61</v>
@@ -13883,8 +13883,8 @@
       <c r="J205" t="s">
         <v>60</v>
       </c>
-      <c r="K205" t="s">
-        <v>30</v>
+      <c r="K205">
+        <v>3</v>
       </c>
       <c r="L205" t="s">
         <v>30</v>
@@ -13893,19 +13893,19 @@
         <v>30</v>
       </c>
       <c r="N205">
-        <v>-0.20420550840019699</v>
+        <v>-0.20420543722777701</v>
       </c>
       <c r="O205">
         <v>1096</v>
       </c>
       <c r="P205">
-        <v>-2.8857876574579202</v>
+        <v>-2.8857874339467799</v>
       </c>
       <c r="Q205">
-        <v>2.4773766406575199</v>
+        <v>2.47737655949122</v>
       </c>
       <c r="R205">
-        <v>1.36815415768251E-2</v>
+        <v>1.36815407995867E-2</v>
       </c>
       <c r="S205" t="s">
         <v>61</v>
@@ -13945,8 +13945,8 @@
       <c r="J206" t="s">
         <v>60</v>
       </c>
-      <c r="K206" t="s">
-        <v>30</v>
+      <c r="K206">
+        <v>1</v>
       </c>
       <c r="L206" t="s">
         <v>30</v>
@@ -13955,19 +13955,19 @@
         <v>30</v>
       </c>
       <c r="N206">
-        <v>-2.47727899099822</v>
+        <v>-2.47727824472355</v>
       </c>
       <c r="O206">
         <v>311</v>
       </c>
       <c r="P206">
-        <v>-6.7138875883651297</v>
+        <v>-6.7138862368981798</v>
       </c>
       <c r="Q206">
-        <v>1.7593296063686901</v>
+        <v>1.7593297474510701</v>
       </c>
       <c r="R206">
-        <v>2.1615349986565901E-2</v>
+        <v>2.1615346898850099E-2</v>
       </c>
       <c r="S206" t="s">
         <v>61</v>
@@ -14007,8 +14007,8 @@
       <c r="J207" t="s">
         <v>60</v>
       </c>
-      <c r="K207" t="s">
-        <v>30</v>
+      <c r="K207">
+        <v>5</v>
       </c>
       <c r="L207" t="s">
         <v>30</v>
@@ -14017,19 +14017,19 @@
         <v>30</v>
       </c>
       <c r="N207">
-        <v>3.2069215913249698</v>
+        <v>3.2069206364081801</v>
       </c>
       <c r="O207">
         <v>278</v>
       </c>
       <c r="P207">
-        <v>-1.17732544446099</v>
+        <v>-1.1773257284673599</v>
       </c>
       <c r="Q207">
-        <v>7.5911686271109398</v>
+        <v>7.5911670012837096</v>
       </c>
       <c r="R207">
-        <v>2.2368607325438598E-2</v>
+        <v>2.2368603902426201E-2</v>
       </c>
       <c r="S207" t="s">
         <v>61</v>
@@ -14069,8 +14069,8 @@
       <c r="J208" t="s">
         <v>60</v>
       </c>
-      <c r="K208" t="s">
-        <v>30</v>
+      <c r="K208">
+        <v>2</v>
       </c>
       <c r="L208" t="s">
         <v>30</v>
@@ -14079,19 +14079,19 @@
         <v>30</v>
       </c>
       <c r="N208">
-        <v>-0.76672888639671699</v>
+        <v>-0.76672855883112601</v>
       </c>
       <c r="O208">
         <v>167</v>
       </c>
       <c r="P208">
-        <v>-5.7717481858381596</v>
+        <v>-5.7717468590561802</v>
       </c>
       <c r="Q208">
-        <v>4.2382904130447301</v>
+        <v>4.2382897413939302</v>
       </c>
       <c r="R208">
-        <v>2.55358127522523E-2</v>
+        <v>2.5535807654209399E-2</v>
       </c>
       <c r="S208" t="s">
         <v>61</v>
@@ -14131,8 +14131,8 @@
       <c r="J209" t="s">
         <v>60</v>
       </c>
-      <c r="K209" t="s">
-        <v>30</v>
+      <c r="K209">
+        <v>5</v>
       </c>
       <c r="L209" t="s">
         <v>30</v>
@@ -14141,19 +14141,19 @@
         <v>30</v>
       </c>
       <c r="N209">
-        <v>4.7214845964019103</v>
+        <v>4.7214828609185497</v>
       </c>
       <c r="O209">
         <v>195</v>
       </c>
       <c r="P209">
-        <v>-0.10559197325143201</v>
+        <v>-0.105592812585639</v>
       </c>
       <c r="Q209">
-        <v>9.5485611660552507</v>
+        <v>9.5485585344227406</v>
       </c>
       <c r="R209">
-        <v>2.46279416819048E-2</v>
+        <v>2.4627937109715298E-2</v>
       </c>
       <c r="S209" t="s">
         <v>61</v>
@@ -14193,8 +14193,8 @@
       <c r="J210" t="s">
         <v>60</v>
       </c>
-      <c r="K210" t="s">
-        <v>30</v>
+      <c r="K210">
+        <v>2</v>
       </c>
       <c r="L210" t="s">
         <v>30</v>
@@ -14203,19 +14203,19 @@
         <v>30</v>
       </c>
       <c r="N210">
-        <v>-1.30746876308215</v>
+        <v>-1.3074683563654199</v>
       </c>
       <c r="O210">
         <v>322</v>
       </c>
       <c r="P210">
-        <v>-5.5397008819831504</v>
+        <v>-5.5396998719538404</v>
       </c>
       <c r="Q210">
-        <v>2.9247633558188402</v>
+        <v>2.9247631592230001</v>
       </c>
       <c r="R210">
-        <v>2.1593021014801001E-2</v>
+        <v>2.1593017936675601E-2</v>
       </c>
       <c r="S210" t="s">
         <v>61</v>
@@ -14255,8 +14255,8 @@
       <c r="J211" t="s">
         <v>60</v>
       </c>
-      <c r="K211" t="s">
-        <v>30</v>
+      <c r="K211">
+        <v>1</v>
       </c>
       <c r="L211" t="s">
         <v>30</v>
@@ -14265,19 +14265,19 @@
         <v>30</v>
       </c>
       <c r="N211">
-        <v>-2.9161300137808901</v>
+        <v>-2.9161291066876101</v>
       </c>
       <c r="O211">
         <v>289</v>
       </c>
       <c r="P211">
-        <v>-7.2432223702782998</v>
+        <v>-7.24322081825132</v>
       </c>
       <c r="Q211">
-        <v>1.4109623427165101</v>
+        <v>1.4109626048760999</v>
       </c>
       <c r="R211">
-        <v>2.2077001818864302E-2</v>
+        <v>2.20769985283863E-2</v>
       </c>
       <c r="S211" t="s">
         <v>61</v>
@@ -14317,8 +14317,8 @@
       <c r="J212" t="s">
         <v>60</v>
       </c>
-      <c r="K212" t="s">
-        <v>30</v>
+      <c r="K212">
+        <v>1</v>
       </c>
       <c r="L212" t="s">
         <v>30</v>
@@ -14327,19 +14327,19 @@
         <v>30</v>
       </c>
       <c r="N212">
-        <v>-2.7369119994839401</v>
+        <v>-2.7369108284083201</v>
       </c>
       <c r="O212">
         <v>152</v>
       </c>
       <c r="P212">
-        <v>-7.8539910325931697</v>
+        <v>-7.8539887935090098</v>
       </c>
       <c r="Q212">
-        <v>2.3801670336252898</v>
+        <v>2.38016713669237</v>
       </c>
       <c r="R212">
-        <v>2.6107546087291999E-2</v>
+        <v>2.6107540638268801E-2</v>
       </c>
       <c r="S212" t="s">
         <v>61</v>
@@ -14379,8 +14379,8 @@
       <c r="J213" t="s">
         <v>60</v>
       </c>
-      <c r="K213" t="s">
-        <v>30</v>
+      <c r="K213">
+        <v>5</v>
       </c>
       <c r="L213" t="s">
         <v>30</v>
@@ -14389,19 +14389,19 @@
         <v>30</v>
       </c>
       <c r="N213">
-        <v>2.7868592138636301</v>
+        <v>2.78685860595363</v>
       </c>
       <c r="O213">
         <v>447</v>
       </c>
       <c r="P213">
-        <v>-0.99253666093248505</v>
+        <v>-0.992536839742861</v>
       </c>
       <c r="Q213">
-        <v>6.5662550886597497</v>
+        <v>6.5662540516501204</v>
       </c>
       <c r="R213">
-        <v>1.9282632014265898E-2</v>
+        <v>1.9282629824982099E-2</v>
       </c>
       <c r="S213" t="s">
         <v>61</v>
@@ -14441,8 +14441,8 @@
       <c r="J214" t="s">
         <v>60</v>
       </c>
-      <c r="K214" t="s">
-        <v>30</v>
+      <c r="K214">
+        <v>3</v>
       </c>
       <c r="L214" t="s">
         <v>30</v>
@@ -14451,19 +14451,19 @@
         <v>30</v>
       </c>
       <c r="N214">
-        <v>-0.39199948534017698</v>
+        <v>-0.39199933026853101</v>
       </c>
       <c r="O214">
         <v>281</v>
       </c>
       <c r="P214">
-        <v>-4.8007385952954102</v>
+        <v>-4.8007377579718797</v>
       </c>
       <c r="Q214">
-        <v>4.0167396246150497</v>
+        <v>4.0167390974348196</v>
       </c>
       <c r="R214">
-        <v>2.2493566887526701E-2</v>
+        <v>2.2493563406649701E-2</v>
       </c>
       <c r="S214" t="s">
         <v>61</v>
@@ -14503,8 +14503,8 @@
       <c r="J215" t="s">
         <v>60</v>
       </c>
-      <c r="K215" t="s">
-        <v>30</v>
+      <c r="K215">
+        <v>1</v>
       </c>
       <c r="L215" t="s">
         <v>30</v>
@@ -14513,19 +14513,19 @@
         <v>30</v>
       </c>
       <c r="N215">
-        <v>-3.3901835593733298</v>
+        <v>-3.3901825032231199</v>
       </c>
       <c r="O215">
         <v>282</v>
       </c>
       <c r="P215">
-        <v>-7.7408174402251397</v>
+        <v>-7.7408157285243</v>
       </c>
       <c r="Q215">
-        <v>0.96045032147847098</v>
+        <v>0.96045072207805504</v>
       </c>
       <c r="R215">
-        <v>2.2197111636999001E-2</v>
+        <v>2.2197108292353E-2</v>
       </c>
       <c r="S215" t="s">
         <v>61</v>
@@ -14565,8 +14565,8 @@
       <c r="J216" t="s">
         <v>60</v>
       </c>
-      <c r="K216" t="s">
-        <v>30</v>
+      <c r="K216">
+        <v>4</v>
       </c>
       <c r="L216" t="s">
         <v>30</v>
@@ -14575,19 +14575,19 @@
         <v>30</v>
       </c>
       <c r="N216">
-        <v>0.45549187760651899</v>
+        <v>0.45549183643323499</v>
       </c>
       <c r="O216">
         <v>602</v>
       </c>
       <c r="P216">
-        <v>-2.9401857586812099</v>
+        <v>-2.9401854890914501</v>
       </c>
       <c r="Q216">
-        <v>3.8511695138942499</v>
+        <v>3.85116916195792</v>
       </c>
       <c r="R216">
-        <v>1.7324885899427201E-2</v>
+        <v>1.7324884313901501E-2</v>
       </c>
       <c r="S216" t="s">
         <v>61</v>
@@ -14627,8 +14627,8 @@
       <c r="J217" t="s">
         <v>60</v>
       </c>
-      <c r="K217" t="s">
-        <v>30</v>
+      <c r="K217">
+        <v>2</v>
       </c>
       <c r="L217" t="s">
         <v>30</v>
@@ -14637,19 +14637,19 @@
         <v>30</v>
       </c>
       <c r="N217">
-        <v>-1.0083656062203901</v>
+        <v>-1.00836534175866</v>
       </c>
       <c r="O217">
         <v>464</v>
       </c>
       <c r="P217">
-        <v>-4.7419319217069198</v>
+        <v>-4.7419312436301597</v>
       </c>
       <c r="Q217">
-        <v>2.7252007092661499</v>
+        <v>2.72520056011283</v>
       </c>
       <c r="R217">
-        <v>1.9048807732074201E-2</v>
+        <v>1.9048805621793299E-2</v>
       </c>
       <c r="S217" t="s">
         <v>61</v>
@@ -14689,8 +14689,8 @@
       <c r="J218" t="s">
         <v>60</v>
       </c>
-      <c r="K218" t="s">
-        <v>30</v>
+      <c r="K218">
+        <v>3</v>
       </c>
       <c r="L218" t="s">
         <v>30</v>
@@ -14699,19 +14699,19 @@
         <v>30</v>
       </c>
       <c r="N218">
-        <v>-0.23578204216270099</v>
+        <v>-0.23578195105251801</v>
       </c>
       <c r="O218">
         <v>464</v>
       </c>
       <c r="P218">
-        <v>-3.9905268906337201</v>
+        <v>-3.9905263787998799</v>
       </c>
       <c r="Q218">
-        <v>3.5189628063083198</v>
+        <v>3.5189624766948402</v>
       </c>
       <c r="R218">
-        <v>1.9156861471790899E-2</v>
+        <v>1.9156859325241599E-2</v>
       </c>
       <c r="S218" t="s">
         <v>61</v>
@@ -14751,8 +14751,8 @@
       <c r="J219" t="s">
         <v>60</v>
       </c>
-      <c r="K219" t="s">
-        <v>30</v>
+      <c r="K219">
+        <v>5</v>
       </c>
       <c r="L219" t="s">
         <v>30</v>
@@ -14761,19 +14761,19 @@
         <v>30</v>
       </c>
       <c r="N219">
-        <v>29.245525855645301</v>
+        <v>29.245524907083499</v>
       </c>
       <c r="O219">
         <v>346</v>
       </c>
       <c r="P219">
-        <v>24.452335320130999</v>
+        <v>24.452334417171699</v>
       </c>
       <c r="Q219">
-        <v>34.038716391159603</v>
+        <v>34.0387153969953</v>
       </c>
       <c r="R219">
-        <v>2.4455053752624099</v>
+        <v>2.4455053519958199</v>
       </c>
       <c r="S219" t="s">
         <v>31</v>
@@ -14813,8 +14813,8 @@
       <c r="J220" t="s">
         <v>60</v>
       </c>
-      <c r="K220" t="s">
-        <v>30</v>
+      <c r="K220">
+        <v>4</v>
       </c>
       <c r="L220" t="s">
         <v>30</v>
@@ -14823,19 +14823,19 @@
         <v>30</v>
       </c>
       <c r="N220">
-        <v>26.284576220533701</v>
+        <v>26.2845760940431</v>
       </c>
       <c r="O220">
         <v>477</v>
       </c>
       <c r="P220">
-        <v>22.3343082738518</v>
+        <v>22.3343081534771</v>
       </c>
       <c r="Q220">
-        <v>30.234844167215499</v>
+        <v>30.2348440346091</v>
       </c>
       <c r="R220">
-        <v>2.01544282993971</v>
+        <v>2.01544282681939</v>
       </c>
       <c r="S220" t="s">
         <v>31</v>
@@ -14875,8 +14875,8 @@
       <c r="J221" t="s">
         <v>60</v>
       </c>
-      <c r="K221" t="s">
-        <v>30</v>
+      <c r="K221">
+        <v>5</v>
       </c>
       <c r="L221" t="s">
         <v>30</v>
@@ -14885,19 +14885,19 @@
         <v>30</v>
       </c>
       <c r="N221">
-        <v>29.869020415789301</v>
+        <v>29.869018813098101</v>
       </c>
       <c r="O221">
         <v>176</v>
       </c>
       <c r="P221">
-        <v>23.107175905455001</v>
+        <v>23.107174406911401</v>
       </c>
       <c r="Q221">
-        <v>36.6308649261236</v>
+        <v>36.630863219284898</v>
       </c>
       <c r="R221">
-        <v>3.44992066853791</v>
+        <v>3.4499206154014002</v>
       </c>
       <c r="S221" t="s">
         <v>31</v>
@@ -14937,8 +14937,8 @@
       <c r="J222" t="s">
         <v>60</v>
       </c>
-      <c r="K222" t="s">
-        <v>30</v>
+      <c r="K222">
+        <v>2</v>
       </c>
       <c r="L222" t="s">
         <v>30</v>
@@ -14947,19 +14947,19 @@
         <v>30</v>
       </c>
       <c r="N222">
-        <v>24.3737417870956</v>
+        <v>24.373742518957901</v>
       </c>
       <c r="O222">
         <v>99</v>
       </c>
       <c r="P222">
-        <v>15.9163610230329</v>
+        <v>15.916361668844299</v>
       </c>
       <c r="Q222">
-        <v>32.831122551158202</v>
+        <v>32.831123369071499</v>
       </c>
       <c r="R222">
-        <v>4.3149901857462396</v>
+        <v>4.31499022964978</v>
       </c>
       <c r="S222" t="s">
         <v>31</v>
@@ -14999,8 +14999,8 @@
       <c r="J223" t="s">
         <v>60</v>
       </c>
-      <c r="K223" t="s">
-        <v>30</v>
+      <c r="K223">
+        <v>2</v>
       </c>
       <c r="L223" t="s">
         <v>30</v>
@@ -15009,19 +15009,19 @@
         <v>30</v>
       </c>
       <c r="N223">
-        <v>24.4525415982407</v>
+        <v>24.452542209543498</v>
       </c>
       <c r="O223">
         <v>133</v>
       </c>
       <c r="P223">
-        <v>17.1478449828228</v>
+        <v>17.1478455323719</v>
       </c>
       <c r="Q223">
-        <v>31.757238213658599</v>
+        <v>31.757238886715001</v>
       </c>
       <c r="R223">
-        <v>3.72688602827444</v>
+        <v>3.7268860597813802</v>
       </c>
       <c r="S223" t="s">
         <v>31</v>
@@ -15061,8 +15061,8 @@
       <c r="J224" t="s">
         <v>60</v>
       </c>
-      <c r="K224" t="s">
-        <v>30</v>
+      <c r="K224">
+        <v>1</v>
       </c>
       <c r="L224" t="s">
         <v>30</v>
@@ -15071,19 +15071,19 @@
         <v>30</v>
       </c>
       <c r="N224">
-        <v>22.469904080055699</v>
+        <v>22.469904848465401</v>
       </c>
       <c r="O224">
         <v>430</v>
       </c>
       <c r="P224">
-        <v>18.524807738000298</v>
+        <v>18.524808458504499</v>
       </c>
       <c r="Q224">
-        <v>26.415000422111</v>
+        <v>26.415001238426399</v>
       </c>
       <c r="R224">
-        <v>2.0128042561506798</v>
+        <v>2.0128042805923299</v>
       </c>
       <c r="S224" t="s">
         <v>31</v>
@@ -15123,8 +15123,8 @@
       <c r="J225" t="s">
         <v>60</v>
       </c>
-      <c r="K225" t="s">
-        <v>30</v>
+      <c r="K225">
+        <v>4</v>
       </c>
       <c r="L225" t="s">
         <v>30</v>
@@ -15133,19 +15133,19 @@
         <v>30</v>
       </c>
       <c r="N225">
-        <v>27.248353704485499</v>
+        <v>27.248353218637099</v>
       </c>
       <c r="O225">
         <v>248</v>
       </c>
       <c r="P225">
-        <v>21.7069246465643</v>
+        <v>21.7069241916154</v>
       </c>
       <c r="Q225">
-        <v>32.789782762406801</v>
+        <v>32.789782245658799</v>
       </c>
       <c r="R225">
-        <v>2.8272597234292101</v>
+        <v>2.8272597076641302</v>
       </c>
       <c r="S225" t="s">
         <v>31</v>
@@ -15185,8 +15185,8 @@
       <c r="J226" t="s">
         <v>60</v>
       </c>
-      <c r="K226" t="s">
-        <v>30</v>
+      <c r="K226">
+        <v>2</v>
       </c>
       <c r="L226" t="s">
         <v>30</v>
@@ -15195,19 +15195,19 @@
         <v>30</v>
       </c>
       <c r="N226">
-        <v>24.381269067505698</v>
+        <v>24.381269503731001</v>
       </c>
       <c r="O226">
         <v>275</v>
       </c>
       <c r="P226">
-        <v>19.306309689049701</v>
+        <v>19.306310094512899</v>
       </c>
       <c r="Q226">
-        <v>29.456228445961699</v>
+        <v>29.456228912949001</v>
       </c>
       <c r="R226">
-        <v>2.58926498900817</v>
+        <v>2.5892650047030998</v>
       </c>
       <c r="S226" t="s">
         <v>31</v>
@@ -15247,8 +15247,8 @@
       <c r="J227" t="s">
         <v>60</v>
       </c>
-      <c r="K227" t="s">
-        <v>30</v>
+      <c r="K227">
+        <v>1</v>
       </c>
       <c r="L227" t="s">
         <v>30</v>
@@ -15257,19 +15257,19 @@
         <v>30</v>
       </c>
       <c r="N227">
-        <v>22.243472188070601</v>
+        <v>22.243472946463601</v>
       </c>
       <c r="O227">
         <v>485</v>
       </c>
       <c r="P227">
-        <v>18.5421667762947</v>
+        <v>18.542167489639699</v>
       </c>
       <c r="Q227">
-        <v>25.944777599846599</v>
+        <v>25.9447784032876</v>
       </c>
       <c r="R227">
-        <v>1.8884211284571299</v>
+        <v>1.8884211514407701</v>
       </c>
       <c r="S227" t="s">
         <v>31</v>
@@ -15309,8 +15309,8 @@
       <c r="J228" t="s">
         <v>60</v>
       </c>
-      <c r="K228" t="s">
-        <v>30</v>
+      <c r="K228">
+        <v>3</v>
       </c>
       <c r="L228" t="s">
         <v>30</v>
@@ -15319,19 +15319,19 @@
         <v>30</v>
       </c>
       <c r="N228">
-        <v>25.662033886673001</v>
+        <v>25.662033933483102</v>
       </c>
       <c r="O228">
         <v>224</v>
       </c>
       <c r="P228">
-        <v>19.942206319014002</v>
+        <v>19.9422063624082</v>
       </c>
       <c r="Q228">
-        <v>31.381861454331901</v>
+        <v>31.3818615045579</v>
       </c>
       <c r="R228">
-        <v>2.9182793712545601</v>
+        <v>2.9182793729973699</v>
       </c>
       <c r="S228" t="s">
         <v>31</v>
@@ -15371,8 +15371,8 @@
       <c r="J229" t="s">
         <v>60</v>
       </c>
-      <c r="K229" t="s">
-        <v>30</v>
+      <c r="K229">
+        <v>2</v>
       </c>
       <c r="L229" t="s">
         <v>30</v>
@@ -15381,19 +15381,19 @@
         <v>30</v>
       </c>
       <c r="N229">
-        <v>24.256972816330201</v>
+        <v>24.256973412063601</v>
       </c>
       <c r="O229">
         <v>189</v>
       </c>
       <c r="P229">
-        <v>18.145937420577798</v>
+        <v>18.145937965302199</v>
       </c>
       <c r="Q229">
-        <v>30.3680082120826</v>
+        <v>30.3680088588251</v>
       </c>
       <c r="R229">
-        <v>3.1178752019145102</v>
+        <v>3.1178752279395301</v>
       </c>
       <c r="S229" t="s">
         <v>31</v>
@@ -15433,8 +15433,8 @@
       <c r="J230" t="s">
         <v>60</v>
       </c>
-      <c r="K230" t="s">
-        <v>30</v>
+      <c r="K230">
+        <v>4</v>
       </c>
       <c r="L230" t="s">
         <v>30</v>
@@ -15443,19 +15443,19 @@
         <v>30</v>
       </c>
       <c r="N230">
-        <v>26.230077383836701</v>
+        <v>26.230077257699701</v>
       </c>
       <c r="O230">
         <v>352</v>
       </c>
       <c r="P230">
-        <v>21.634668182574099</v>
+        <v>21.634668063557701</v>
       </c>
       <c r="Q230">
-        <v>30.825486585099299</v>
+        <v>30.825486451841599</v>
       </c>
       <c r="R230">
-        <v>2.3445965312564101</v>
+        <v>2.3445965276234499</v>
       </c>
       <c r="S230" t="s">
         <v>31</v>
@@ -15495,8 +15495,8 @@
       <c r="J231" t="s">
         <v>60</v>
       </c>
-      <c r="K231" t="s">
-        <v>30</v>
+      <c r="K231">
+        <v>4</v>
       </c>
       <c r="L231" t="s">
         <v>30</v>
@@ -15505,19 +15505,19 @@
         <v>30</v>
       </c>
       <c r="N231">
-        <v>27.045048574403499</v>
+        <v>27.0450482240967</v>
       </c>
       <c r="O231">
         <v>333</v>
       </c>
       <c r="P231">
-        <v>22.274094634084701</v>
+        <v>22.274094303222</v>
       </c>
       <c r="Q231">
-        <v>31.816002514722399</v>
+        <v>31.816002144971399</v>
       </c>
       <c r="R231">
-        <v>2.43416017363205</v>
+        <v>2.4341601637116002</v>
       </c>
       <c r="S231" t="s">
         <v>31</v>
@@ -15557,8 +15557,8 @@
       <c r="J232" t="s">
         <v>60</v>
       </c>
-      <c r="K232" t="s">
-        <v>30</v>
+      <c r="K232">
+        <v>3</v>
       </c>
       <c r="L232" t="s">
         <v>30</v>
@@ -15567,19 +15567,19 @@
         <v>30</v>
       </c>
       <c r="N232">
-        <v>25.563327956430101</v>
+        <v>25.5633279849059</v>
       </c>
       <c r="O232">
         <v>542</v>
       </c>
       <c r="P232">
-        <v>21.890855070583299</v>
+        <v>21.890855097716202</v>
       </c>
       <c r="Q232">
-        <v>29.235800842276799</v>
+        <v>29.235800872095702</v>
       </c>
       <c r="R232">
-        <v>1.87371065604426</v>
+        <v>1.8737106567294599</v>
       </c>
       <c r="S232" t="s">
         <v>31</v>
@@ -15619,8 +15619,8 @@
       <c r="J233" t="s">
         <v>60</v>
       </c>
-      <c r="K233" t="s">
-        <v>30</v>
+      <c r="K233">
+        <v>2</v>
       </c>
       <c r="L233" t="s">
         <v>30</v>
@@ -15629,19 +15629,19 @@
         <v>30</v>
       </c>
       <c r="N233">
-        <v>24.367804672560101</v>
+        <v>24.367804979119001</v>
       </c>
       <c r="O233">
         <v>483</v>
       </c>
       <c r="P233">
-        <v>20.5391688220943</v>
+        <v>20.5391691123295</v>
       </c>
       <c r="Q233">
-        <v>28.1964405230258</v>
+        <v>28.196440845908601</v>
       </c>
       <c r="R233">
-        <v>1.9533856379927399</v>
+        <v>1.9533856463212</v>
       </c>
       <c r="S233" t="s">
         <v>31</v>
@@ -15681,8 +15681,8 @@
       <c r="J234" t="s">
         <v>60</v>
       </c>
-      <c r="K234" t="s">
-        <v>30</v>
+      <c r="K234">
+        <v>1</v>
       </c>
       <c r="L234" t="s">
         <v>30</v>
@@ -15691,19 +15691,19 @@
         <v>30</v>
       </c>
       <c r="N234">
-        <v>22.1900467098767</v>
+        <v>22.190047645962501</v>
       </c>
       <c r="O234">
         <v>356</v>
       </c>
       <c r="P234">
-        <v>17.873586340545799</v>
+        <v>17.8735872115513</v>
       </c>
       <c r="Q234">
-        <v>26.506507079207498</v>
+        <v>26.506508080373699</v>
       </c>
       <c r="R234">
-        <v>2.2022756986381702</v>
+        <v>2.2022757318424602</v>
       </c>
       <c r="S234" t="s">
         <v>31</v>
@@ -15743,8 +15743,8 @@
       <c r="J235" t="s">
         <v>60</v>
       </c>
-      <c r="K235" t="s">
-        <v>30</v>
+      <c r="K235">
+        <v>4</v>
       </c>
       <c r="L235" t="s">
         <v>30</v>
@@ -15753,19 +15753,19 @@
         <v>30</v>
       </c>
       <c r="N235">
-        <v>27.223039510054299</v>
+        <v>27.2230390496822</v>
       </c>
       <c r="O235">
         <v>264</v>
       </c>
       <c r="P235">
-        <v>21.853718476240498</v>
+        <v>21.853718044286399</v>
       </c>
       <c r="Q235">
-        <v>32.592360543867997</v>
+        <v>32.592360055077897</v>
       </c>
       <c r="R235">
-        <v>2.73944950704783</v>
+        <v>2.73944949254884</v>
       </c>
       <c r="S235" t="s">
         <v>31</v>
@@ -15805,8 +15805,8 @@
       <c r="J236" t="s">
         <v>60</v>
       </c>
-      <c r="K236" t="s">
-        <v>30</v>
+      <c r="K236">
+        <v>3</v>
       </c>
       <c r="L236" t="s">
         <v>30</v>
@@ -15815,19 +15815,19 @@
         <v>30</v>
       </c>
       <c r="N236">
-        <v>25.819383383943698</v>
+        <v>25.819383396591</v>
       </c>
       <c r="O236">
         <v>69</v>
       </c>
       <c r="P236">
-        <v>15.492965909634499</v>
+        <v>15.492965920633001</v>
       </c>
       <c r="Q236">
-        <v>36.145800858252898</v>
+        <v>36.145800872549003</v>
       </c>
       <c r="R236">
-        <v>5.2685803440352998</v>
+        <v>5.2685803448765398</v>
       </c>
       <c r="S236" t="s">
         <v>31</v>
@@ -15867,8 +15867,8 @@
       <c r="J237" t="s">
         <v>60</v>
       </c>
-      <c r="K237" t="s">
-        <v>30</v>
+      <c r="K237">
+        <v>5</v>
       </c>
       <c r="L237" t="s">
         <v>30</v>
@@ -15877,19 +15877,19 @@
         <v>30</v>
       </c>
       <c r="N237">
-        <v>33.873615673174498</v>
+        <v>33.873612719614798</v>
       </c>
       <c r="O237">
         <v>211</v>
       </c>
       <c r="P237">
-        <v>27.487555446491001</v>
+        <v>27.487552628724998</v>
       </c>
       <c r="Q237">
-        <v>40.259675899857903</v>
+        <v>40.259672810504497</v>
       </c>
       <c r="R237">
-        <v>3.2581939932058401</v>
+        <v>3.2581939239233701</v>
       </c>
       <c r="S237" t="s">
         <v>31</v>
@@ -15929,8 +15929,8 @@
       <c r="J238" t="s">
         <v>60</v>
       </c>
-      <c r="K238" t="s">
-        <v>30</v>
+      <c r="K238">
+        <v>5</v>
       </c>
       <c r="L238" t="s">
         <v>30</v>
@@ -15939,19 +15939,19 @@
         <v>30</v>
       </c>
       <c r="N238">
-        <v>30.033089150282301</v>
+        <v>30.033087063341</v>
       </c>
       <c r="O238">
         <v>102</v>
       </c>
       <c r="P238">
-        <v>21.1369342169106</v>
+        <v>21.136932306382398</v>
       </c>
       <c r="Q238">
-        <v>38.929244083653998</v>
+        <v>38.929241820299602</v>
       </c>
       <c r="R238">
-        <v>4.5388545578426802</v>
+        <v>4.5388544678360097</v>
       </c>
       <c r="S238" t="s">
         <v>31</v>
@@ -15991,8 +15991,8 @@
       <c r="J239" t="s">
         <v>60</v>
       </c>
-      <c r="K239" t="s">
-        <v>30</v>
+      <c r="K239">
+        <v>3</v>
       </c>
       <c r="L239" t="s">
         <v>30</v>
@@ -16001,19 +16001,19 @@
         <v>30</v>
       </c>
       <c r="N239">
-        <v>25.670111311675399</v>
+        <v>25.670111338785301</v>
       </c>
       <c r="O239">
         <v>322</v>
       </c>
       <c r="P239">
-        <v>20.898953817879502</v>
+        <v>20.898953843339999</v>
       </c>
       <c r="Q239">
-        <v>30.441268805471399</v>
+        <v>30.441268834230598</v>
       </c>
       <c r="R239">
-        <v>2.4342640274469298</v>
+        <v>2.43426402828841</v>
       </c>
       <c r="S239" t="s">
         <v>31</v>
@@ -16053,8 +16053,8 @@
       <c r="J240" t="s">
         <v>60</v>
       </c>
-      <c r="K240" t="s">
-        <v>30</v>
+      <c r="K240">
+        <v>3</v>
       </c>
       <c r="L240" t="s">
         <v>30</v>
@@ -16063,19 +16063,19 @@
         <v>30</v>
       </c>
       <c r="N240">
-        <v>25.7947783910673</v>
+        <v>25.7947783879574</v>
       </c>
       <c r="O240">
         <v>328</v>
       </c>
       <c r="P240">
-        <v>21.059971366531499</v>
+        <v>21.059971363607801</v>
       </c>
       <c r="Q240">
-        <v>30.529585415603201</v>
+        <v>30.5295854123071</v>
       </c>
       <c r="R240">
-        <v>2.4157178696611399</v>
+        <v>2.4157178695661399</v>
       </c>
       <c r="S240" t="s">
         <v>31</v>
@@ -16115,8 +16115,8 @@
       <c r="J241" t="s">
         <v>60</v>
       </c>
-      <c r="K241" t="s">
-        <v>30</v>
+      <c r="K241">
+        <v>4</v>
       </c>
       <c r="L241" t="s">
         <v>30</v>
@@ -16125,19 +16125,19 @@
         <v>30</v>
       </c>
       <c r="N241">
-        <v>26.414571219652</v>
+        <v>26.414571044881001</v>
       </c>
       <c r="O241">
         <v>364</v>
       </c>
       <c r="P241">
-        <v>21.885354784136201</v>
+        <v>21.8853546189703</v>
       </c>
       <c r="Q241">
-        <v>30.943787655167799</v>
+        <v>30.943787470791801</v>
       </c>
       <c r="R241">
-        <v>2.3108247119978702</v>
+        <v>2.31082470709732</v>
       </c>
       <c r="S241" t="s">
         <v>31</v>
@@ -16177,8 +16177,8 @@
       <c r="J242" t="s">
         <v>60</v>
       </c>
-      <c r="K242" t="s">
-        <v>30</v>
+      <c r="K242">
+        <v>1</v>
       </c>
       <c r="L242" t="s">
         <v>30</v>
@@ -16187,19 +16187,19 @@
         <v>30</v>
       </c>
       <c r="N242">
-        <v>22.841851260393099</v>
+        <v>22.841852476362401</v>
       </c>
       <c r="O242">
         <v>161</v>
       </c>
       <c r="P242">
-        <v>16.357005030369699</v>
+        <v>16.357006124829802</v>
       </c>
       <c r="Q242">
-        <v>29.3266974904165</v>
+        <v>29.326698827895001</v>
       </c>
       <c r="R242">
-        <v>3.3085950153180601</v>
+        <v>3.3085950773125701</v>
       </c>
       <c r="S242" t="s">
         <v>31</v>
@@ -16239,8 +16239,8 @@
       <c r="J243" t="s">
         <v>60</v>
       </c>
-      <c r="K243" t="s">
-        <v>30</v>
+      <c r="K243">
+        <v>4</v>
       </c>
       <c r="L243" t="s">
         <v>30</v>
@@ -16249,19 +16249,19 @@
         <v>30</v>
       </c>
       <c r="N243">
-        <v>28.073149622700502</v>
+        <v>28.073148909615298</v>
       </c>
       <c r="O243">
         <v>273</v>
       </c>
       <c r="P243">
-        <v>22.742675496452701</v>
+        <v>22.742674824643899</v>
       </c>
       <c r="Q243">
-        <v>33.403623748948398</v>
+        <v>33.403622994586797</v>
       </c>
       <c r="R243">
-        <v>2.7196296562488902</v>
+        <v>2.7196296351895199</v>
       </c>
       <c r="S243" t="s">
         <v>31</v>
@@ -16301,8 +16301,8 @@
       <c r="J244" t="s">
         <v>60</v>
       </c>
-      <c r="K244" t="s">
-        <v>30</v>
+      <c r="K244">
+        <v>1</v>
       </c>
       <c r="L244" t="s">
         <v>30</v>
@@ -16311,19 +16311,19 @@
         <v>30</v>
       </c>
       <c r="N244">
-        <v>24.1528929415947</v>
+        <v>24.152893802905201</v>
       </c>
       <c r="O244">
         <v>89</v>
       </c>
       <c r="P244">
-        <v>15.2605714331422</v>
+        <v>15.260572186389201</v>
       </c>
       <c r="Q244">
-        <v>33.045214450047297</v>
+        <v>33.045215419421197</v>
       </c>
       <c r="R244">
-        <v>4.5368987288023401</v>
+        <v>4.5368987839367296</v>
       </c>
       <c r="S244" t="s">
         <v>31</v>
@@ -16363,8 +16363,8 @@
       <c r="J245" t="s">
         <v>60</v>
       </c>
-      <c r="K245" t="s">
-        <v>30</v>
+      <c r="K245">
+        <v>5</v>
       </c>
       <c r="L245" t="s">
         <v>30</v>
@@ -16373,19 +16373,19 @@
         <v>30</v>
       </c>
       <c r="N245">
-        <v>30.0458845809557</v>
+        <v>30.045882957629999</v>
       </c>
       <c r="O245">
         <v>185</v>
       </c>
       <c r="P245">
-        <v>23.439416529947501</v>
+        <v>23.4394150084362</v>
       </c>
       <c r="Q245">
-        <v>36.652352631963801</v>
+        <v>36.652350906823699</v>
       </c>
       <c r="R245">
-        <v>3.3706469648000801</v>
+        <v>3.37064691285395</v>
       </c>
       <c r="S245" t="s">
         <v>31</v>
@@ -16425,8 +16425,8 @@
       <c r="J246" t="s">
         <v>60</v>
       </c>
-      <c r="K246" t="s">
-        <v>30</v>
+      <c r="K246">
+        <v>3</v>
       </c>
       <c r="L246" t="s">
         <v>30</v>
@@ -16435,19 +16435,19 @@
         <v>30</v>
       </c>
       <c r="N246">
-        <v>25.779564357749301</v>
+        <v>25.7795643378584</v>
       </c>
       <c r="O246">
         <v>1096</v>
       </c>
       <c r="P246">
-        <v>23.189859145537898</v>
+        <v>23.189859126299002</v>
       </c>
       <c r="Q246">
-        <v>28.3692695699608</v>
+        <v>28.369269549417801</v>
       </c>
       <c r="R246">
-        <v>1.3212781694956399</v>
+        <v>1.32127816916296</v>
       </c>
       <c r="S246" t="s">
         <v>31</v>
@@ -16487,8 +16487,8 @@
       <c r="J247" t="s">
         <v>60</v>
       </c>
-      <c r="K247" t="s">
-        <v>30</v>
+      <c r="K247">
+        <v>1</v>
       </c>
       <c r="L247" t="s">
         <v>30</v>
@@ -16497,19 +16497,19 @@
         <v>30</v>
       </c>
       <c r="N247">
-        <v>23.5064908751513</v>
+        <v>23.506491530362599</v>
       </c>
       <c r="O247">
         <v>311</v>
       </c>
       <c r="P247">
-        <v>18.793657669796499</v>
+        <v>18.793658279510002</v>
       </c>
       <c r="Q247">
-        <v>28.219324080506102</v>
+        <v>28.219324781215199</v>
       </c>
       <c r="R247">
-        <v>2.4045067374258999</v>
+        <v>2.40450676063907</v>
       </c>
       <c r="S247" t="s">
         <v>31</v>
@@ -16549,8 +16549,8 @@
       <c r="J248" t="s">
         <v>60</v>
       </c>
-      <c r="K248" t="s">
-        <v>30</v>
+      <c r="K248">
+        <v>5</v>
       </c>
       <c r="L248" t="s">
         <v>30</v>
@@ -16559,19 +16559,19 @@
         <v>30</v>
       </c>
       <c r="N248">
-        <v>29.1906914574745</v>
+        <v>29.190690411494302</v>
       </c>
       <c r="O248">
         <v>278</v>
       </c>
       <c r="P248">
-        <v>23.8462657863248</v>
+        <v>23.8462647966237</v>
       </c>
       <c r="Q248">
-        <v>34.5351171286243</v>
+        <v>34.535116026364904</v>
       </c>
       <c r="R248">
-        <v>2.7267477914029299</v>
+        <v>2.7267477626890901</v>
       </c>
       <c r="S248" t="s">
         <v>31</v>
@@ -16611,8 +16611,8 @@
       <c r="J249" t="s">
         <v>60</v>
       </c>
-      <c r="K249" t="s">
-        <v>30</v>
+      <c r="K249">
+        <v>2</v>
       </c>
       <c r="L249" t="s">
         <v>30</v>
@@ -16621,19 +16621,19 @@
         <v>30</v>
       </c>
       <c r="N249">
-        <v>25.217040979752799</v>
+        <v>25.217041216255002</v>
       </c>
       <c r="O249">
         <v>167</v>
       </c>
       <c r="P249">
-        <v>18.630669519099001</v>
+        <v>18.630669735130301</v>
       </c>
       <c r="Q249">
-        <v>31.8034124404066</v>
+        <v>31.803412697379802</v>
       </c>
       <c r="R249">
-        <v>3.3603936023743901</v>
+        <v>3.3603936128187502</v>
       </c>
       <c r="S249" t="s">
         <v>31</v>
@@ -16673,8 +16673,8 @@
       <c r="J250" t="s">
         <v>60</v>
       </c>
-      <c r="K250" t="s">
-        <v>30</v>
+      <c r="K250">
+        <v>5</v>
       </c>
       <c r="L250" t="s">
         <v>30</v>
@@ -16683,19 +16683,19 @@
         <v>30</v>
       </c>
       <c r="N250">
-        <v>30.705254462551402</v>
+        <v>30.705252636004701</v>
       </c>
       <c r="O250">
         <v>195</v>
       </c>
       <c r="P250">
-        <v>24.230917956833299</v>
+        <v>24.2309162375253</v>
       </c>
       <c r="Q250">
-        <v>37.179590968269601</v>
+        <v>37.179589034484003</v>
       </c>
       <c r="R250">
-        <v>3.3032329110807099</v>
+        <v>3.3032328563670101</v>
       </c>
       <c r="S250" t="s">
         <v>31</v>
@@ -16735,8 +16735,8 @@
       <c r="J251" t="s">
         <v>60</v>
       </c>
-      <c r="K251" t="s">
-        <v>30</v>
+      <c r="K251">
+        <v>2</v>
       </c>
       <c r="L251" t="s">
         <v>30</v>
@@ -16745,19 +16745,19 @@
         <v>30</v>
       </c>
       <c r="N251">
-        <v>24.676301103067399</v>
+        <v>24.676301418720701</v>
       </c>
       <c r="O251">
         <v>322</v>
       </c>
       <c r="P251">
-        <v>19.967243691457401</v>
+        <v>19.967243986859099</v>
       </c>
       <c r="Q251">
-        <v>29.385358514677399</v>
+        <v>29.385358850582399</v>
       </c>
       <c r="R251">
-        <v>2.4025803120459299</v>
+        <v>2.4025803223783901</v>
       </c>
       <c r="S251" t="s">
         <v>31</v>
@@ -16797,8 +16797,8 @@
       <c r="J252" t="s">
         <v>60</v>
       </c>
-      <c r="K252" t="s">
-        <v>30</v>
+      <c r="K252">
+        <v>1</v>
       </c>
       <c r="L252" t="s">
         <v>30</v>
@@ -16807,19 +16807,19 @@
         <v>30</v>
       </c>
       <c r="N252">
-        <v>23.0676398523686</v>
+        <v>23.0676406683985</v>
       </c>
       <c r="O252">
         <v>289</v>
       </c>
       <c r="P252">
-        <v>18.210694029471401</v>
+        <v>18.210694785351802</v>
       </c>
       <c r="Q252">
-        <v>27.924585675265899</v>
+        <v>27.924586551445199</v>
       </c>
       <c r="R252">
-        <v>2.4780335831108502</v>
+        <v>2.47803361379933</v>
       </c>
       <c r="S252" t="s">
         <v>31</v>
@@ -16859,8 +16859,8 @@
       <c r="J253" t="s">
         <v>60</v>
       </c>
-      <c r="K253" t="s">
-        <v>30</v>
+      <c r="K253">
+        <v>1</v>
       </c>
       <c r="L253" t="s">
         <v>30</v>
@@ -16869,19 +16869,19 @@
         <v>30</v>
       </c>
       <c r="N253">
-        <v>23.2468578666656</v>
+        <v>23.246858946677801</v>
       </c>
       <c r="O253">
         <v>152</v>
       </c>
       <c r="P253">
-        <v>16.5315722429477</v>
+        <v>16.531573214215399</v>
       </c>
       <c r="Q253">
-        <v>29.9621434903835</v>
+        <v>29.962144679140199</v>
       </c>
       <c r="R253">
-        <v>3.4261661345499399</v>
+        <v>3.4261661900318598</v>
       </c>
       <c r="S253" t="s">
         <v>31</v>
@@ -16921,8 +16921,8 @@
       <c r="J254" t="s">
         <v>60</v>
       </c>
-      <c r="K254" t="s">
-        <v>30</v>
+      <c r="K254">
+        <v>5</v>
       </c>
       <c r="L254" t="s">
         <v>30</v>
@@ -16931,19 +16931,19 @@
         <v>30</v>
       </c>
       <c r="N254">
-        <v>28.770629080013201</v>
+        <v>28.770628381039799</v>
       </c>
       <c r="O254">
         <v>447</v>
       </c>
       <c r="P254">
-        <v>24.573942431854</v>
+        <v>24.573941763268099</v>
       </c>
       <c r="Q254">
-        <v>32.967315728172302</v>
+        <v>32.967314998811403</v>
       </c>
       <c r="R254">
-        <v>2.14116665722407</v>
+        <v>2.14116664172021</v>
       </c>
       <c r="S254" t="s">
         <v>31</v>
@@ -16983,8 +16983,8 @@
       <c r="J255" t="s">
         <v>60</v>
       </c>
-      <c r="K255" t="s">
-        <v>30</v>
+      <c r="K255">
+        <v>3</v>
       </c>
       <c r="L255" t="s">
         <v>30</v>
@@ -16993,19 +16993,19 @@
         <v>30</v>
       </c>
       <c r="N255">
-        <v>25.5917703808094</v>
+        <v>25.591770444817602</v>
       </c>
       <c r="O255">
         <v>281</v>
       </c>
       <c r="P255">
-        <v>20.489498904079198</v>
+        <v>20.489498963901301</v>
       </c>
       <c r="Q255">
-        <v>30.694041857539499</v>
+        <v>30.694041925733899</v>
       </c>
       <c r="R255">
-        <v>2.6031997330255798</v>
+        <v>2.6031997351613598</v>
       </c>
       <c r="S255" t="s">
         <v>31</v>
@@ -17045,8 +17045,8 @@
       <c r="J256" t="s">
         <v>60</v>
       </c>
-      <c r="K256" t="s">
-        <v>30</v>
+      <c r="K256">
+        <v>1</v>
       </c>
       <c r="L256" t="s">
         <v>30</v>
@@ -17055,19 +17055,19 @@
         <v>30</v>
       </c>
       <c r="N256">
-        <v>22.593586306776199</v>
+        <v>22.593587271863001</v>
       </c>
       <c r="O256">
         <v>282</v>
       </c>
       <c r="P256">
-        <v>17.712543945811198</v>
+        <v>17.712544837078799</v>
       </c>
       <c r="Q256">
-        <v>27.4746286677412</v>
+        <v>27.4746297066472</v>
       </c>
       <c r="R256">
-        <v>2.4903277351862498</v>
+        <v>2.49032777284908</v>
       </c>
       <c r="S256" t="s">
         <v>31</v>
@@ -17107,8 +17107,8 @@
       <c r="J257" t="s">
         <v>60</v>
       </c>
-      <c r="K257" t="s">
-        <v>30</v>
+      <c r="K257">
+        <v>4</v>
       </c>
       <c r="L257" t="s">
         <v>30</v>
@@ -17117,19 +17117,19 @@
         <v>30</v>
       </c>
       <c r="N257">
-        <v>26.439261743756099</v>
+        <v>26.439261611519399</v>
       </c>
       <c r="O257">
         <v>602</v>
       </c>
       <c r="P257">
-        <v>22.9163194660503</v>
+        <v>22.9163193394571</v>
       </c>
       <c r="Q257">
-        <v>29.962204021461901</v>
+        <v>29.962203883581601</v>
       </c>
       <c r="R257">
-        <v>1.7974195294417299</v>
+        <v>1.79741952656238</v>
       </c>
       <c r="S257" t="s">
         <v>31</v>
@@ -17169,8 +17169,8 @@
       <c r="J258" t="s">
         <v>60</v>
       </c>
-      <c r="K258" t="s">
-        <v>30</v>
+      <c r="K258">
+        <v>2</v>
       </c>
       <c r="L258" t="s">
         <v>30</v>
@@ -17179,19 +17179,19 @@
         <v>30</v>
       </c>
       <c r="N258">
-        <v>24.975404259929199</v>
+        <v>24.975404433327501</v>
       </c>
       <c r="O258">
         <v>464</v>
       </c>
       <c r="P258">
-        <v>21.0366836428101</v>
+        <v>21.036683807087201</v>
       </c>
       <c r="Q258">
-        <v>28.914124877048199</v>
+        <v>28.914125059567699</v>
       </c>
       <c r="R258">
-        <v>2.00955133526484</v>
+        <v>2.0095513399185099</v>
       </c>
       <c r="S258" t="s">
         <v>31</v>
@@ -17231,8 +17231,8 @@
       <c r="J259" t="s">
         <v>60</v>
       </c>
-      <c r="K259" t="s">
-        <v>30</v>
+      <c r="K259">
+        <v>3</v>
       </c>
       <c r="L259" t="s">
         <v>30</v>
@@ -17241,19 +17241,19 @@
         <v>30</v>
       </c>
       <c r="N259">
-        <v>25.747987823986801</v>
+        <v>25.747987824033601</v>
       </c>
       <c r="O259">
         <v>464</v>
       </c>
       <c r="P259">
-        <v>21.769455945699001</v>
+        <v>21.769455945743399</v>
       </c>
       <c r="Q259">
-        <v>29.7265197022747</v>
+        <v>29.726519702323799</v>
       </c>
       <c r="R259">
-        <v>2.0298632032080799</v>
+        <v>2.0298632032092798</v>
       </c>
       <c r="S259" t="s">
         <v>31</v>

</xml_diff>